<commit_message>
ptit commit master - pour vider le master
</commit_message>
<xml_diff>
--- a/ProjetConnect/donneesUsers.xlsx
+++ b/ProjetConnect/donneesUsers.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
@@ -599,6 +599,60 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>mgrael</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>enkwudhu</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>rmgraelenkwudhu@gmail.com</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>YTWYRlMctmNuilk</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>17-02-2022 08:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>fzydmi</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>hieekebs</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>yfzydmihieekebs@gmail.com</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>fnxeFuwmIyFxwAf</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>17-02-2022 08:14</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>